<commit_message>
Chrome driver update, added more defects, code cleanup
</commit_message>
<xml_diff>
--- a/src/test/resources/files/TCs and Defects.xlsx
+++ b/src/test/resources/files/TCs and Defects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="495" windowWidth="23655" windowHeight="9405"/>
+    <workbookView xWindow="240" yWindow="495" windowWidth="23655" windowHeight="9405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
   <si>
     <t>ID</t>
   </si>
@@ -341,17 +341,60 @@
     <t>It is possible to enter negative quantity of pizzas as well as letters and special symbols</t>
   </si>
   <si>
-    <t>Message "Please, provide valid quantity" should be shown. Cost field value should not be re-calculated</t>
+    <t>Confirmation message with total cost as negative or NaN is shown</t>
   </si>
   <si>
-    <t>Confirmation message with total cost as negative or NaN is shown</t>
+    <t>It is possible to place order when numbers with decimal point are specified in Quantity field</t>
+  </si>
+  <si>
+    <t>Cost field value is re-calculated. Pop-up window with confirmation message is shown</t>
+  </si>
+  <si>
+    <t>Message "Please, provide valid quantity" should be shown when invalid data is specified in Quantity field. Cost field value should not be re-calculated</t>
+  </si>
+  <si>
+    <t>Message "Please, provide valid quantity" should be shown when invalid data is specified in Quantity field. Cost field value should not be re-calculated.</t>
+  </si>
+  <si>
+    <t>1. Open Pizza Order Form page
+2. Select any Pizza Type, Topping 1 and Topping 2 options.
+3. Try to type any negative number into Quantity input field, e.g. "-2"
+4. Fill in Name and Phone input fields
+5. Select payment option
+6. Click Place Order button</t>
+  </si>
+  <si>
+    <t>1. Open Pizza Order Form page
+2. Select any Pizza Type, Topping 1 and Topping 2 options.
+3. Try to type any negative number into Quantity input field, e.g. "-2"
+4. Try to type any letter into Quantity input field, e.g. "2f"
+5. Try to type any special character into Quantity input field, e.g. "1*"
+6. Fill in Name and Phone input fields
+7. Select payment option
+8. Click Place Order button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Pizza Order Form page
+2. Select Pizza Type with 1 or 2 toppings
+3. Do not select Topping 1 and Topping 2 options.
+3. Fill in Quantity input field with any valid value, e.g. "1"
+4. Fill in Name and Phone input fields
+5. Select payment option
+6. Click Place Order button
+</t>
+  </si>
+  <si>
+    <t>Message "Please, select toppings options" should be shown</t>
+  </si>
+  <si>
+    <t>Pizzas with 1 or 2 toppings can be ordered while no topping options have been selected in drop-downs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -376,6 +419,26 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="6">
@@ -437,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -517,8 +580,17 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,7 +804,7 @@
   </sheetPr>
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -5016,10 +5088,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G998"/>
+  <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5064,7 +5136,7 @@
       <c r="C2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="31" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -5126,57 +5198,89 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>72</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="29" t="s">
         <v>74</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>66</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="89.25">
+    <row r="6" spans="1:7" ht="153">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="29" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="D6" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="102">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="12.75">
-      <c r="A7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:7" ht="12.75">
-      <c r="A8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="E8" s="13"/>
+      <c r="C7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="127.5">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="6"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="7"/>
       <c r="E9" s="13"/>
     </row>
@@ -10125,12 +10229,18 @@
       <c r="C998" s="7"/>
       <c r="E998" s="13"/>
     </row>
+    <row r="999" spans="1:5" ht="12.75">
+      <c r="A999" s="6"/>
+      <c r="C999" s="7"/>
+      <c r="E999" s="13"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="C2:C998">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C999">
       <formula1>"LOW,MEDIUM,HIGH,CRITICAL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more test cases added
</commit_message>
<xml_diff>
--- a/src/test/resources/files/TCs and Defects.xlsx
+++ b/src/test/resources/files/TCs and Defects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="495" windowWidth="23655" windowHeight="9405" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="495" windowWidth="23655" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -107,20 +107,7 @@
     <t>Verify valiation message on Quantity input field</t>
   </si>
   <si>
-    <t>1. Open Pizza Order Form page
-2. Try to type any negative number into Quantity input field, e.g. "-2"
-3. Try to type any letter into Quantity input field, e.g. "2f"
-4. Try to type any special character into Quantity input field, e.g. "1*"</t>
-  </si>
-  <si>
-    <t>1. Default value of Quantity input field should be 0, maximum available value should be 5-numbers long
-2-4 Message "Please, provide valid quantity" should be shown. Cost field value should not be re-calculated</t>
-  </si>
-  <si>
     <t>Failed</t>
-  </si>
-  <si>
-    <t>Defect #5</t>
   </si>
   <si>
     <t>Verify Name field is mandatory</t>
@@ -388,6 +375,47 @@
   </si>
   <si>
     <t>Pizzas with 1 or 2 toppings can be ordered while no topping options have been selected in drop-downs</t>
+  </si>
+  <si>
+    <t>Defect #5, 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Pizza Order Form page
+2. Try to type any negative number into Quantity input field, e.g. "-2"
+3. Try to type any numbers with decimal point into Quantity input field, e.g. "1*"
+4. Try to type any letter into Quantity input field, e.g. "2f"
+5. Try to type any special character into Quantity input field, e.g. "1*"
+</t>
+  </si>
+  <si>
+    <t>1. Default value of Quantity input field should be 0, maximum available value should be 5-numbers long
+2-5 Message "Please, provide valid quantity" should be shown. Cost field value should not be re-calculated</t>
+  </si>
+  <si>
+    <t>Verify pizza with toppings can not be ordered without toppings options selected</t>
+  </si>
+  <si>
+    <t>User name = Natallia
+User phone number = +12345678900</t>
+  </si>
+  <si>
+    <t>Defect #7</t>
+  </si>
+  <si>
+    <t>1. Open Pizza Order Form page
+2. Select Pizza Type with 1 or 2 toppings, do not select Topping 1 and Topping 2 options.
+3. Fill in Quantity input field with any valid value, e.g. "1"
+4. Fill in Name and Phone input fields
+5. Select any payment option
+6. Click Place Order button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Page with Pizza Order Form title should be opened
+2. Chosen pizza type should be displayed as selected. It should be possible to change the choice
+3. Cost field value should be calculated correctly and be in format "##.##". Cost value should be disabled for editing. Cost should be re-calculate in case another Pizza Type or Quantity is specified
+4. User name and phone should be displayed as specified
+5. Payment option shoud be displayed as selected
+6. Message "Please, select toppings options" should be shown </t>
   </si>
 </sst>
 </file>
@@ -802,9 +830,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H1001"/>
+  <dimension ref="A1:H1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -864,7 +894,7 @@
     </row>
     <row r="3" spans="1:8" ht="165.75">
       <c r="A3" s="19">
-        <f t="shared" ref="A3:A13" si="0">A2+1</f>
+        <f t="shared" ref="A3:A14" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -904,7 +934,7 @@
       </c>
       <c r="H4" s="20"/>
     </row>
-    <row r="5" spans="1:8" ht="51">
+    <row r="5" spans="1:8" ht="89.25">
       <c r="A5" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -914,42 +944,42 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="21" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="23" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="51">
       <c r="A6" s="19">
-        <f t="shared" si="0"/>
+        <f>A5+1</f>
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="51">
@@ -958,23 +988,23 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.5">
@@ -983,15 +1013,15 @@
         <v>7</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G8" s="26" t="s">
         <v>11</v>
@@ -1004,21 +1034,21 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="140.25">
@@ -1027,107 +1057,125 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" ht="76.5">
+    <row r="11" spans="1:8" ht="114.75">
       <c r="A11" s="19">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="25.5">
+        <v>19</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="76.5">
       <c r="A12" s="19">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>47</v>
+      <c r="B12" s="21" t="s">
+        <v>40</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="21"/>
+        <v>41</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>38</v>
+      </c>
       <c r="F12" s="21" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="51">
+        <v>19</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="25.5">
       <c r="A13" s="19">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C13" s="20"/>
-      <c r="D13" s="28" t="s">
-        <v>52</v>
+      <c r="D13" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="21" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H13" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="51">
+      <c r="A14" s="19">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="12.75">
-      <c r="A14" s="4"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="G14" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="12.75">
-      <c r="A15" s="6"/>
-      <c r="G15" s="7"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="12.75">
       <c r="A16" s="6"/>
@@ -5073,9 +5121,13 @@
       <c r="A1001" s="6"/>
       <c r="G1001" s="7"/>
     </row>
+    <row r="1002" spans="1:7" ht="12.75">
+      <c r="A1002" s="6"/>
+      <c r="G1002" s="7"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="G2:G1001">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G1002">
       <formula1>"Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5090,8 +5142,8 @@
   </sheetPr>
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5105,22 +5157,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
@@ -5131,19 +5183,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="G2" s="4"/>
     </row>
@@ -5153,19 +5205,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -5175,22 +5227,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="G4" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="114.75">
@@ -5199,19 +5251,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="F5" s="29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -5221,19 +5273,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -5242,19 +5294,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -5263,19 +5315,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75">

</xml_diff>